<commit_message>
fix(dict): changed isMissing value to 'FALSE' instead of '0'
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
+++ b/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14230423-40C0-6C4D-84FC-2195F320556B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E8306B-C1D4-F543-8968-3079EB8697D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3690,6 +3690,7 @@
     <font>
       <sz val="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -4275,7 +4276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG598"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -12783,12 +12784,13 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="14.1640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -12813,7 +12815,7 @@
       <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -12827,7 +12829,7 @@
       <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -12841,7 +12843,7 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -12855,7 +12857,7 @@
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -12869,7 +12871,7 @@
       <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -12883,7 +12885,7 @@
       <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -12897,7 +12899,7 @@
       <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -12911,7 +12913,7 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -12925,7 +12927,7 @@
       <c r="B10" s="3">
         <v>0</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -12939,7 +12941,7 @@
       <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -12953,7 +12955,7 @@
       <c r="B12" s="3">
         <v>0</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -12967,7 +12969,7 @@
       <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -12981,7 +12983,7 @@
       <c r="B14" s="3">
         <v>0</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -12995,7 +12997,7 @@
       <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -13009,7 +13011,7 @@
       <c r="B16" s="3">
         <v>0</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -13023,7 +13025,7 @@
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -13037,7 +13039,7 @@
       <c r="B18" s="3">
         <v>0</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -13051,7 +13053,7 @@
       <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -13065,7 +13067,7 @@
       <c r="B20" s="3">
         <v>0</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -13079,7 +13081,7 @@
       <c r="B21" s="3">
         <v>1</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -13093,7 +13095,7 @@
       <c r="B22" s="3">
         <v>0</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -13107,7 +13109,7 @@
       <c r="B23" s="3">
         <v>1</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -13121,7 +13123,7 @@
       <c r="B24" s="3">
         <v>0</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -13135,7 +13137,7 @@
       <c r="B25" s="3">
         <v>1</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -13149,7 +13151,7 @@
       <c r="B26" s="3">
         <v>0</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -13163,7 +13165,7 @@
       <c r="B27" s="3">
         <v>1</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -13177,7 +13179,7 @@
       <c r="B28" s="3">
         <v>0</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -13191,7 +13193,7 @@
       <c r="B29" s="3">
         <v>1</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -13205,7 +13207,7 @@
       <c r="B30" s="3">
         <v>0</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -13219,7 +13221,7 @@
       <c r="B31" s="3">
         <v>1</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -13233,7 +13235,7 @@
       <c r="B32" s="3">
         <v>0</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -13247,7 +13249,7 @@
       <c r="B33" s="3">
         <v>1</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -13261,7 +13263,7 @@
       <c r="B34" s="3">
         <v>0</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -13275,7 +13277,7 @@
       <c r="B35" s="3">
         <v>1</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -13289,7 +13291,7 @@
       <c r="B36" s="3">
         <v>0</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -13303,7 +13305,7 @@
       <c r="B37" s="3">
         <v>1</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -13317,7 +13319,7 @@
       <c r="B38" s="3">
         <v>0</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -13331,7 +13333,7 @@
       <c r="B39" s="3">
         <v>1</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -13345,7 +13347,7 @@
       <c r="B40" s="3">
         <v>0</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -13359,7 +13361,7 @@
       <c r="B41" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -13373,7 +13375,7 @@
       <c r="B42" s="3">
         <v>0</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="4" t="s">
@@ -13387,7 +13389,7 @@
       <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -13401,7 +13403,7 @@
       <c r="B44" s="3">
         <v>0</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="4" t="s">
@@ -13415,7 +13417,7 @@
       <c r="B45" s="3">
         <v>1</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -13429,7 +13431,7 @@
       <c r="B46" s="3">
         <v>0</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="4" t="s">
@@ -13443,7 +13445,7 @@
       <c r="B47" s="3">
         <v>1</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="5" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="4" t="s">

</xml_diff>

<commit_message>
fix: updated asthma_current_CHICOS to asthma_current_ISAAC and pets_pregn to pets_preg
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
+++ b/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8DB56D-34F0-DA49-A5B6-F6683AD7BBD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477670E4-0E9B-2E4E-BEAC-9CF7A8A3A490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="92">
   <si>
     <t>name</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>asthma_current_ISAAC</t>
+  </si>
+  <si>
+    <t>pets_preg</t>
   </si>
 </sst>
 </file>
@@ -901,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1343,7 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>34</v>
@@ -1469,7 +1475,7 @@
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
fix: updated fake data WP5 and updated categories WP5
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
+++ b/R/data/dictionaries/outcome/1_0/1_0_non_repeated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477670E4-0E9B-2E4E-BEAC-9CF7A8A3A490}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126A91C-43C3-8C47-BAA6-A6856229D8A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -212,9 +212,6 @@
     <t>Current asthma (MeDALL)</t>
   </si>
   <si>
-    <t>asthma_current_CHICOS</t>
-  </si>
-  <si>
     <t>Current asthma (ISAAC)</t>
   </si>
   <si>
@@ -276,9 +273,6 @@
   </si>
   <si>
     <t>Ever diagnosis of COPD in adulthood based on physician diagnosis</t>
-  </si>
-  <si>
-    <t>pets_pregn</t>
   </si>
   <si>
     <t>Furry pet (dogs, cats, rodents) ownership in child's household during pregnancy.</t>
@@ -907,7 +901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -1007,7 +1001,7 @@
         <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9" t="s">
@@ -1343,146 +1337,146 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1499,13 +1493,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="14.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.5" style="1" customWidth="1"/>
+    <col min="2" max="4" width="14.1640625" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1534,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1548,7 +1543,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1562,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1576,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1590,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1604,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1618,7 +1613,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1632,7 +1627,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1646,7 +1641,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1660,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1674,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1688,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1716,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1730,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1744,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1758,7 +1753,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1772,7 +1767,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1786,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1800,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1814,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1828,12 +1823,12 @@
         <v>0</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B24" s="3">
         <v>0</v>
@@ -1842,12 +1837,12 @@
         <v>0</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
@@ -1856,12 +1851,12 @@
         <v>0</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3">
         <v>0</v>
@@ -1870,12 +1865,12 @@
         <v>0</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
@@ -1884,12 +1879,12 @@
         <v>0</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="3">
         <v>0</v>
@@ -1898,12 +1893,12 @@
         <v>0</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3">
         <v>1</v>
@@ -1912,12 +1907,12 @@
         <v>0</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3">
         <v>0</v>
@@ -1926,12 +1921,12 @@
         <v>0</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="3">
         <v>1</v>
@@ -1940,12 +1935,12 @@
         <v>0</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3">
         <v>0</v>
@@ -1954,12 +1949,12 @@
         <v>0</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="3">
         <v>1</v>
@@ -1968,12 +1963,12 @@
         <v>0</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B34" s="3">
         <v>0</v>
@@ -1982,12 +1977,12 @@
         <v>0</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B35" s="3">
         <v>1</v>
@@ -1996,12 +1991,12 @@
         <v>0</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" s="3">
         <v>0</v>
@@ -2010,12 +2005,12 @@
         <v>0</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" s="3">
         <v>1</v>
@@ -2024,12 +2019,12 @@
         <v>0</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="3">
         <v>0</v>
@@ -2038,12 +2033,12 @@
         <v>0</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3">
         <v>1</v>
@@ -2052,12 +2047,12 @@
         <v>0</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B40" s="3">
         <v>0</v>
@@ -2066,12 +2061,12 @@
         <v>0</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="3">
         <v>1</v>
@@ -2080,12 +2075,12 @@
         <v>0</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B42" s="3">
         <v>0</v>
@@ -2094,12 +2089,12 @@
         <v>0</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="3">
         <v>1</v>
@@ -2108,12 +2103,12 @@
         <v>0</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B44" s="3">
         <v>0</v>
@@ -2122,12 +2117,12 @@
         <v>0</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="3">
         <v>1</v>
@@ -2136,12 +2131,12 @@
         <v>0</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B46" s="3">
         <v>0</v>
@@ -2150,12 +2145,12 @@
         <v>0</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B47" s="3">
         <v>1</v>
@@ -2164,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>